<commit_message>
clearvars except allSpecies instead of clearAll, changed length to size to deal with cases where number of taxa to include is less than 3, made it so that the evaluation of each cell results in a display indicating completion
</commit_message>
<xml_diff>
--- a/setsOfTaxaAndColors.xlsx
+++ b/setsOfTaxaAndColors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="17235" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="17235" windowHeight="7965" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>Mycetozoa</t>
   </si>
@@ -189,6 +190,30 @@
   </si>
   <si>
     <t>Bony, ray-finned, lung fish</t>
+  </si>
+  <si>
+    <t>Chelicerata</t>
+  </si>
+  <si>
+    <t>Myriapoda</t>
+  </si>
+  <si>
+    <t>Hexapoda</t>
+  </si>
+  <si>
+    <t>Chelicerates</t>
+  </si>
+  <si>
+    <t>Myriapods</t>
+  </si>
+  <si>
+    <t>Crustacea</t>
+  </si>
+  <si>
+    <t>Crustaceans</t>
+  </si>
+  <si>
+    <t>Hexapods (includes insects)</t>
   </si>
 </sst>
 </file>
@@ -610,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -887,7 +912,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -932,4 +957,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2012-03-17-accessionNumbers.txt and dataGeneratorForGenomicMDS.m , merged the capability to display numbers next to points on plot and the lines to write the excel spreadsheet with species info from Sayem's fork (though the latter doesn't work), the legend now displays the number of species from each taxon, and the user can now specify in setsOfTaxaAndColors.xlsx whether or not they want numbers displayed beside the points on the plots for each taxon by a 1 or 0
</commit_message>
<xml_diff>
--- a/setsOfTaxaAndColors.xlsx
+++ b/setsOfTaxaAndColors.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="17235" windowHeight="7965" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="17235" windowHeight="7965" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>Mycetozoa</t>
   </si>
@@ -144,9 +145,6 @@
     <t>Insecta</t>
   </si>
   <si>
-    <t>Insects</t>
-  </si>
-  <si>
     <t>Primates</t>
   </si>
   <si>
@@ -192,28 +190,37 @@
     <t>Bony, ray-finned, lung fish</t>
   </si>
   <si>
-    <t>Chelicerata</t>
-  </si>
-  <si>
-    <t>Myriapoda</t>
-  </si>
-  <si>
-    <t>Hexapoda</t>
-  </si>
-  <si>
-    <t>Chelicerates</t>
-  </si>
-  <si>
-    <t>Myriapods</t>
-  </si>
-  <si>
-    <t>Crustacea</t>
-  </si>
-  <si>
-    <t>Crustaceans</t>
-  </si>
-  <si>
-    <t>Hexapods (includes insects)</t>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Class: Insects</t>
+  </si>
+  <si>
+    <t>Class: Amphibians</t>
+  </si>
+  <si>
+    <t>Diprotodontia</t>
+  </si>
+  <si>
+    <t>Class: Mammals</t>
+  </si>
+  <si>
+    <t>Rodentia</t>
+  </si>
+  <si>
+    <t>Order: Primates (infraclass eutheria , superorder euarchontoglires)</t>
+  </si>
+  <si>
+    <t>Order: Rodents (infraclass eutheria , superorder euarchontoglires)</t>
+  </si>
+  <si>
+    <t>Order: Diprodonts (infraclass metatheria , superorder marsupialia)</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Haplorrhini</t>
   </si>
 </sst>
 </file>
@@ -555,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -567,7 +574,7 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +584,11 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -588,8 +598,11 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -599,8 +612,11 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -610,8 +626,11 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -621,8 +640,11 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
     </row>
   </sheetData>
@@ -633,10 +655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,7 +667,7 @@
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -655,8 +677,11 @@
       <c r="C1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -666,8 +691,11 @@
       <c r="C2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -677,8 +705,11 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -688,8 +719,11 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -699,19 +733,25 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -721,8 +761,11 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -732,8 +775,11 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -743,8 +789,11 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -754,8 +803,11 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -765,8 +817,11 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -776,8 +831,11 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -785,7 +843,10 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -798,45 +859,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -846,10 +920,73 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G6"/>
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="72.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -858,48 +995,60 @@
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -907,12 +1056,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -921,37 +1070,46 @@
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -959,65 +1117,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added column to setsOfTaxaAndColors.xlsx for color of marker edges, adjusted genomicMDS.m to read this new column and to use it appropriately, just about to try to make the legends combine groups of entries into single legend entries
</commit_message>
<xml_diff>
--- a/setsOfTaxaAndColors.xlsx
+++ b/setsOfTaxaAndColors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1485" windowWidth="17235" windowHeight="7635" tabRatio="1000" activeTab="6"/>
+    <workbookView xWindow="1560" yWindow="1485" windowWidth="17235" windowHeight="7635" tabRatio="1000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1-allOrganisms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="97">
   <si>
     <t>Metazoa</t>
   </si>
@@ -696,7 +696,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="D18" sqref="D1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,8 +1009,11 @@
       <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="D1">
-        <v>1</v>
+      <c r="D1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1026,8 +1029,11 @@
       <c r="C2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1043,8 +1049,11 @@
       <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1060,8 +1069,11 @@
       <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1077,8 +1089,11 @@
       <c r="C5" t="s">
         <v>93</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1094,8 +1109,11 @@
       <c r="C6" t="s">
         <v>89</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1111,8 +1129,11 @@
       <c r="C7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1128,8 +1149,11 @@
       <c r="C8" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D8">
-        <v>1</v>
+      <c r="D8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1145,8 +1169,11 @@
       <c r="C9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D9">
-        <v>1</v>
+      <c r="D9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1162,8 +1189,11 @@
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10">
-        <v>1</v>
+      <c r="D10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1179,8 +1209,11 @@
       <c r="C11" t="s">
         <v>90</v>
       </c>
-      <c r="D11">
-        <v>1</v>
+      <c r="D11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1208,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1254,7 @@
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1231,11 +1264,14 @@
       <c r="C1" t="s">
         <v>94</v>
       </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1245,11 +1281,14 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1259,8 +1298,11 @@
       <c r="C3" t="s">
         <v>95</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1270,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,46 +1324,46 @@
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>95</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="E3" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1334,7 +1376,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,8 +1397,11 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="D1">
-        <v>1</v>
+      <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
       </c>
       <c r="F1" s="5"/>
     </row>
@@ -1370,8 +1415,11 @@
       <c r="C2" t="s">
         <v>89</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -1385,8 +1433,11 @@
       <c r="C3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -1400,8 +1451,11 @@
       <c r="C4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
       </c>
       <c r="F4" s="5"/>
     </row>
@@ -1415,8 +1469,11 @@
       <c r="C5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -1430,8 +1487,11 @@
       <c r="C6" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -1445,8 +1505,11 @@
       <c r="C7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="7">
-        <v>1</v>
+      <c r="D7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1459,8 +1522,11 @@
       <c r="C8" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="7">
-        <v>1</v>
+      <c r="D8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1473,8 +1539,11 @@
       <c r="C9" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="7">
-        <v>1</v>
+      <c r="D9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1556,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1637,7 @@
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>87</v>
       </c>
@@ -1578,11 +1647,14 @@
       <c r="C1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
@@ -1592,8 +1664,11 @@
       <c r="C2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="7">
-        <v>1</v>
+      <c r="D2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1603,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1690,7 @@
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>59</v>
       </c>
@@ -1629,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>60</v>
       </c>
@@ -1643,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>61</v>
       </c>
@@ -1657,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>62</v>
       </c>
@@ -1671,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>81</v>
       </c>
@@ -1685,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>64</v>
       </c>
@@ -1699,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>65</v>
       </c>
@@ -1709,11 +1784,14 @@
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>66</v>
       </c>
@@ -1723,11 +1801,14 @@
       <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>67</v>
       </c>
@@ -1737,11 +1818,14 @@
       <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>68</v>
       </c>
@@ -1751,11 +1835,14 @@
       <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>69</v>
       </c>
@@ -1765,11 +1852,14 @@
       <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>70</v>
       </c>
@@ -1779,11 +1869,14 @@
       <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>71</v>
       </c>
@@ -1793,11 +1886,14 @@
       <c r="C13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>72</v>
       </c>
@@ -1807,11 +1903,14 @@
       <c r="C14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>73</v>
       </c>
@@ -1821,11 +1920,14 @@
       <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>74</v>
       </c>
@@ -1835,11 +1937,14 @@
       <c r="C16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>75</v>
       </c>
@@ -1849,11 +1954,14 @@
       <c r="C17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>76</v>
       </c>
@@ -1863,11 +1971,14 @@
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>77</v>
       </c>
@@ -1877,11 +1988,14 @@
       <c r="C19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>78</v>
       </c>
@@ -1891,11 +2005,14 @@
       <c r="C20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>79</v>
       </c>
@@ -1905,8 +2022,11 @@
       <c r="C21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="6">
-        <v>1</v>
+      <c r="D21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2014 November 21. This code generates Figures 1 to 7 of "Mapping the Space of Genomic Signatures" by Lila Kari, Kathleen A. Hill, Abu S. Sayem, Rallis Karamichalis, Nathaniel Bryans, Katelyn Davis, and Nikesh S. Dattani
</commit_message>
<xml_diff>
--- a/setsOfTaxaAndColors.xlsx
+++ b/setsOfTaxaAndColors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1605" windowWidth="15795" windowHeight="6540" tabRatio="1000" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="1560" yWindow="1605" windowWidth="15795" windowHeight="6540" tabRatio="1000" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-CGRfigures" sheetId="1" r:id="rId1"/>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,12 +1666,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>